<commit_message>
Week 2 (Started): Project Plan Updated
Signed-off-by: Ahmed-Zoher <59732468+Ahmed-Zoher@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8D0810-324E-4172-AA95-31A1C184E075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEF645B-9921-4BD4-A41F-E727883092FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Ahmed Zoher</t>
-  </si>
-  <si>
-    <t>OVERALL PROGRESS</t>
   </si>
   <si>
     <t>TASK NAME</t>
@@ -221,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -272,37 +269,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -324,9 +295,6 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -369,24 +337,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -640,11 +595,11 @@
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF1003"/>
+  <dimension ref="A1:AF1002"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -710,11 +665,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -749,11 +704,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -783,11 +738,11 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -806,105 +761,105 @@
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
     </row>
-    <row r="5" spans="1:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:32" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+    </row>
+    <row r="6" spans="1:32" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-    </row>
-    <row r="6" spans="1:32" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-    </row>
-    <row r="7" spans="1:32" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="5"/>
+    </row>
+    <row r="7" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="14" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -929,18 +884,34 @@
     </row>
     <row r="8" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="15" t="s">
-        <v>32</v>
+      <c r="B8" s="16" t="s">
+        <v>15</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="C8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="18">
+        <v>43851</v>
+      </c>
+      <c r="F8" s="19">
+        <v>43852</v>
+      </c>
+      <c r="G8" s="19">
+        <v>43854</v>
+      </c>
+      <c r="H8" s="19">
+        <v>43854</v>
+      </c>
+      <c r="I8" s="23">
+        <v>3</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="16"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -963,36 +934,36 @@
       <c r="AE8" s="3"/>
       <c r="AF8" s="5"/>
     </row>
-    <row r="9" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>17</v>
+      <c r="D9" s="16" t="s">
+        <v>27</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="E9" s="18">
+        <v>43852</v>
+      </c>
+      <c r="F9" s="19">
+        <v>43854</v>
+      </c>
+      <c r="G9" s="19">
+        <v>43854</v>
+      </c>
+      <c r="H9" s="19">
+        <v>43855</v>
+      </c>
+      <c r="I9" s="23">
+        <v>3</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="19">
-        <v>43851</v>
-      </c>
-      <c r="F9" s="20">
-        <v>43852</v>
-      </c>
-      <c r="G9" s="20">
-        <v>43854</v>
-      </c>
-      <c r="H9" s="20">
-        <v>43854</v>
-      </c>
-      <c r="I9" s="24">
-        <v>3</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="17"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -1015,36 +986,36 @@
       <c r="AE9" s="3"/>
       <c r="AF9" s="5"/>
     </row>
-    <row r="10" spans="1:32" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="17" t="s">
-        <v>18</v>
+      <c r="B10" s="16" t="s">
+        <v>19</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>17</v>
+      <c r="C10" s="16" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <v>43852</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="19">
         <v>43854</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <v>43854</v>
       </c>
-      <c r="H10" s="20">
-        <v>43855</v>
+      <c r="H10" s="19">
+        <v>43854</v>
       </c>
-      <c r="I10" s="24">
-        <v>3</v>
+      <c r="I10" s="23">
+        <v>2</v>
       </c>
-      <c r="J10" s="17" t="s">
-        <v>22</v>
+      <c r="J10" s="16" t="s">
+        <v>21</v>
       </c>
-      <c r="K10" s="17"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -1069,34 +1040,34 @@
     </row>
     <row r="11" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="17" t="s">
-        <v>20</v>
+      <c r="B11" s="16" t="s">
+        <v>18</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>17</v>
+      <c r="C11" s="16" t="s">
+        <v>16</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>29</v>
+      <c r="D11" s="17" t="s">
+        <v>25</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="18">
         <v>43852</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="19">
         <v>43854</v>
       </c>
-      <c r="G11" s="20">
-        <v>43854</v>
+      <c r="G11" s="19">
+        <v>43855</v>
       </c>
-      <c r="H11" s="20">
-        <v>43854</v>
+      <c r="H11" s="19">
+        <v>43856</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="23">
         <v>2</v>
       </c>
-      <c r="J11" s="17" t="s">
-        <v>22</v>
+      <c r="J11" s="16" t="s">
+        <v>21</v>
       </c>
-      <c r="K11" s="17"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -1122,31 +1093,31 @@
     <row r="12" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>26</v>
+      <c r="D12" s="17" t="s">
+        <v>4</v>
       </c>
       <c r="E12" s="19">
-        <v>43852</v>
-      </c>
-      <c r="F12" s="20">
-        <v>43854</v>
-      </c>
-      <c r="G12" s="20">
         <v>43855</v>
       </c>
-      <c r="H12" s="20">
+      <c r="F12" s="19">
         <v>43856</v>
       </c>
-      <c r="I12" s="24">
-        <v>2</v>
+      <c r="G12" s="19">
+        <v>43855</v>
+      </c>
+      <c r="H12" s="19">
+        <v>43855</v>
+      </c>
+      <c r="I12" s="23">
+        <v>1</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" s="17"/>
       <c r="L12" s="3"/>
@@ -1173,34 +1144,34 @@
     </row>
     <row r="13" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>17</v>
+      <c r="C13" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="19">
+        <v>43854</v>
+      </c>
+      <c r="F13" s="19">
         <v>43855</v>
       </c>
-      <c r="F13" s="20">
-        <v>43856</v>
+      <c r="G13" s="19">
+        <v>43854</v>
       </c>
-      <c r="G13" s="20">
+      <c r="H13" s="19">
         <v>43855</v>
       </c>
-      <c r="H13" s="20">
-        <v>43855</v>
-      </c>
-      <c r="I13" s="24">
+      <c r="I13" s="23">
         <v>1</v>
       </c>
-      <c r="J13" s="18" t="s">
-        <v>22</v>
+      <c r="J13" s="17" t="s">
+        <v>21</v>
       </c>
-      <c r="K13" s="18"/>
+      <c r="K13" s="17"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -1223,36 +1194,36 @@
       <c r="AE13" s="3"/>
       <c r="AF13" s="5"/>
     </row>
-    <row r="14" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>17</v>
+      <c r="C14" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>4</v>
+      <c r="D14" s="17" t="s">
+        <v>26</v>
       </c>
-      <c r="E14" s="20">
-        <v>43854</v>
-      </c>
-      <c r="F14" s="20">
+      <c r="E14" s="19">
         <v>43855</v>
       </c>
-      <c r="G14" s="20">
-        <v>43854</v>
+      <c r="F14" s="19">
+        <v>43856</v>
       </c>
-      <c r="H14" s="20">
+      <c r="G14" s="19">
         <v>43855</v>
       </c>
-      <c r="I14" s="24">
+      <c r="H14" s="19">
+        <v>43855</v>
+      </c>
+      <c r="I14" s="23">
         <v>1</v>
       </c>
-      <c r="J14" s="18" t="s">
-        <v>22</v>
+      <c r="J14" s="17" t="s">
+        <v>21</v>
       </c>
-      <c r="K14" s="18"/>
+      <c r="K14" s="17"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -1275,36 +1246,36 @@
       <c r="AE14" s="3"/>
       <c r="AF14" s="5"/>
     </row>
-    <row r="15" spans="1:32" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="18" t="s">
-        <v>25</v>
+    <row r="15" spans="1:32" s="25" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="17" t="s">
+        <v>29</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>17</v>
+      <c r="C15" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>27</v>
+      <c r="D15" s="17" t="s">
+        <v>26</v>
       </c>
-      <c r="E15" s="20">
-        <v>43855</v>
+      <c r="E15" s="19">
+        <v>43858</v>
       </c>
-      <c r="F15" s="20">
-        <v>43856</v>
+      <c r="F15" s="19">
+        <v>43860</v>
       </c>
-      <c r="G15" s="20">
-        <v>43855</v>
+      <c r="G15" s="19">
+        <v>43858</v>
       </c>
-      <c r="H15" s="20">
-        <v>43855</v>
+      <c r="H15" s="19">
+        <v>43862</v>
       </c>
-      <c r="I15" s="24">
-        <v>1</v>
+      <c r="I15" s="23">
+        <v>3</v>
       </c>
-      <c r="J15" s="18" t="s">
-        <v>22</v>
+      <c r="J15" s="17" t="s">
+        <v>21</v>
       </c>
-      <c r="K15" s="18"/>
+      <c r="K15" s="17"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -1327,36 +1298,20 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="5"/>
     </row>
-    <row r="16" spans="1:32" s="26" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="18" t="s">
-        <v>30</v>
+    <row r="16" spans="1:32" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="14" t="s">
+        <v>32</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="20">
-        <v>43858</v>
-      </c>
-      <c r="F16" s="20">
-        <v>43860</v>
-      </c>
-      <c r="G16" s="20">
-        <v>43858</v>
-      </c>
-      <c r="H16" s="20">
-        <v>43862</v>
-      </c>
-      <c r="I16" s="24">
-        <v>3</v>
-      </c>
-      <c r="J16" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="18"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -1379,20 +1334,30 @@
       <c r="AE16" s="3"/>
       <c r="AF16" s="5"/>
     </row>
-    <row r="17" spans="1:32" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="15" t="s">
-        <v>33</v>
+    <row r="17" spans="1:32" s="27" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="17" t="s">
+        <v>22</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
+      <c r="C17" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="19">
+        <v>43863</v>
+      </c>
+      <c r="F17" s="19">
+        <v>43864</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="17"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -1415,30 +1380,30 @@
       <c r="AE17" s="3"/>
       <c r="AF17" s="5"/>
     </row>
-    <row r="18" spans="1:32" s="28" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="18" t="s">
+    <row r="18" spans="1:32" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>17</v>
+      <c r="C18" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>29</v>
+      <c r="D18" s="17" t="s">
+        <v>33</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="19">
         <v>43863</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="19">
         <v>43864</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="18" t="s">
-        <v>31</v>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="17" t="s">
+        <v>30</v>
       </c>
-      <c r="K18" s="18"/>
+      <c r="K18" s="17"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1461,30 +1426,30 @@
       <c r="AE18" s="3"/>
       <c r="AF18" s="5"/>
     </row>
-    <row r="19" spans="1:32" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="18" t="s">
+    <row r="19" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>17</v>
+      <c r="C19" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>34</v>
+      <c r="D19" s="17" t="s">
+        <v>27</v>
       </c>
-      <c r="E19" s="20">
-        <v>43863</v>
+      <c r="E19" s="19">
+        <v>43865</v>
       </c>
-      <c r="F19" s="20">
-        <v>43864</v>
+      <c r="F19" s="19">
+        <v>43835</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="18" t="s">
-        <v>31</v>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="17" t="s">
+        <v>30</v>
       </c>
-      <c r="K19" s="18"/>
+      <c r="K19" s="17"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -1507,30 +1472,30 @@
       <c r="AE19" s="3"/>
       <c r="AF19" s="5"/>
     </row>
-    <row r="20" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="18" t="s">
+    <row r="20" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>17</v>
+      <c r="E20" s="19">
+        <v>43866</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>28</v>
+      <c r="F20" s="19">
+        <v>43867</v>
       </c>
-      <c r="E20" s="20">
-        <v>43865</v>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="17" t="s">
+        <v>30</v>
       </c>
-      <c r="F20" s="20">
-        <v>43835</v>
-      </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K20" s="18"/>
+      <c r="K20" s="17"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -1553,30 +1518,30 @@
       <c r="AE20" s="3"/>
       <c r="AF20" s="5"/>
     </row>
-    <row r="21" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="18" t="s">
-        <v>25</v>
+    <row r="21" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="17" t="s">
+        <v>24</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>17</v>
+      <c r="C21" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>26</v>
+      <c r="D21" s="17" t="s">
+        <v>20</v>
       </c>
-      <c r="E21" s="20">
-        <v>43866</v>
-      </c>
-      <c r="F21" s="20">
+      <c r="E21" s="19">
         <v>43867</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="18" t="s">
-        <v>31</v>
+      <c r="F21" s="19">
+        <v>43868</v>
       </c>
-      <c r="K21" s="18"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="17"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -1599,30 +1564,30 @@
       <c r="AE21" s="3"/>
       <c r="AF21" s="5"/>
     </row>
-    <row r="22" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="18" t="s">
-        <v>25</v>
+    <row r="22" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="17" t="s">
+        <v>34</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>17</v>
+      <c r="C22" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>21</v>
+      <c r="D22" s="17" t="s">
+        <v>4</v>
       </c>
-      <c r="E22" s="20">
-        <v>43867</v>
-      </c>
-      <c r="F22" s="20">
+      <c r="E22" s="19">
         <v>43868</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="18" t="s">
-        <v>31</v>
+      <c r="F22" s="19">
+        <v>43869</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="17"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -1645,30 +1610,30 @@
       <c r="AE22" s="3"/>
       <c r="AF22" s="5"/>
     </row>
-    <row r="23" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="18" t="s">
+    <row r="23" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>17</v>
+      <c r="C23" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="19">
         <v>43868</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="19">
         <v>43869</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="18" t="s">
-        <v>31</v>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="17" t="s">
+        <v>30</v>
       </c>
-      <c r="K23" s="18"/>
+      <c r="K23" s="17"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -1691,30 +1656,18 @@
       <c r="AE23" s="3"/>
       <c r="AF23" s="5"/>
     </row>
-    <row r="24" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="20">
-        <v>43868</v>
-      </c>
-      <c r="F24" s="20">
-        <v>43869</v>
-      </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K24" s="18"/>
+    <row r="24" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -1739,8 +1692,8 @@
     </row>
     <row r="25" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="22"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1773,9 +1726,9 @@
     </row>
     <row r="26" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="23"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -2179,73 +2132,73 @@
       <c r="AE37" s="3"/>
       <c r="AF37" s="5"/>
     </row>
-    <row r="38" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="3"/>
-      <c r="AC38" s="3"/>
-      <c r="AD38" s="3"/>
-      <c r="AE38" s="3"/>
-      <c r="AF38" s="5"/>
-    </row>
-    <row r="39" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+    </row>
+    <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
-      <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-      <c r="AF39" s="1"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="5"/>
     </row>
     <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -8471,37 +8424,37 @@
     </row>
     <row r="223" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
-      <c r="B223" s="3"/>
-      <c r="C223" s="3"/>
-      <c r="D223" s="3"/>
-      <c r="E223" s="3"/>
-      <c r="F223" s="3"/>
-      <c r="G223" s="3"/>
-      <c r="H223" s="3"/>
-      <c r="I223" s="3"/>
-      <c r="J223" s="3"/>
-      <c r="K223" s="3"/>
-      <c r="L223" s="3"/>
-      <c r="M223" s="3"/>
-      <c r="N223" s="3"/>
-      <c r="O223" s="3"/>
-      <c r="P223" s="3"/>
-      <c r="Q223" s="3"/>
-      <c r="R223" s="3"/>
-      <c r="S223" s="3"/>
-      <c r="T223" s="3"/>
-      <c r="U223" s="3"/>
-      <c r="V223" s="3"/>
-      <c r="W223" s="3"/>
-      <c r="X223" s="3"/>
-      <c r="Y223" s="3"/>
-      <c r="Z223" s="3"/>
-      <c r="AA223" s="3"/>
-      <c r="AB223" s="3"/>
-      <c r="AC223" s="3"/>
-      <c r="AD223" s="3"/>
-      <c r="AE223" s="3"/>
-      <c r="AF223" s="5"/>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
+      <c r="D223" s="1"/>
+      <c r="E223" s="1"/>
+      <c r="F223" s="1"/>
+      <c r="G223" s="1"/>
+      <c r="H223" s="1"/>
+      <c r="I223" s="1"/>
+      <c r="J223" s="1"/>
+      <c r="K223" s="1"/>
+      <c r="L223" s="1"/>
+      <c r="M223" s="1"/>
+      <c r="N223" s="1"/>
+      <c r="O223" s="1"/>
+      <c r="P223" s="1"/>
+      <c r="Q223" s="1"/>
+      <c r="R223" s="1"/>
+      <c r="S223" s="1"/>
+      <c r="T223" s="1"/>
+      <c r="U223" s="1"/>
+      <c r="V223" s="1"/>
+      <c r="W223" s="1"/>
+      <c r="X223" s="1"/>
+      <c r="Y223" s="1"/>
+      <c r="Z223" s="1"/>
+      <c r="AA223" s="1"/>
+      <c r="AB223" s="1"/>
+      <c r="AC223" s="1"/>
+      <c r="AD223" s="1"/>
+      <c r="AE223" s="1"/>
+      <c r="AF223" s="1"/>
     </row>
     <row r="224" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
@@ -34989,55 +34942,15 @@
       <c r="AE1002" s="1"/>
       <c r="AF1002" s="1"/>
     </row>
-    <row r="1003" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1003" s="1"/>
-      <c r="B1003" s="1"/>
-      <c r="C1003" s="1"/>
-      <c r="D1003" s="1"/>
-      <c r="E1003" s="1"/>
-      <c r="F1003" s="1"/>
-      <c r="G1003" s="1"/>
-      <c r="H1003" s="1"/>
-      <c r="I1003" s="1"/>
-      <c r="J1003" s="1"/>
-      <c r="K1003" s="1"/>
-      <c r="L1003" s="1"/>
-      <c r="M1003" s="1"/>
-      <c r="N1003" s="1"/>
-      <c r="O1003" s="1"/>
-      <c r="P1003" s="1"/>
-      <c r="Q1003" s="1"/>
-      <c r="R1003" s="1"/>
-      <c r="S1003" s="1"/>
-      <c r="T1003" s="1"/>
-      <c r="U1003" s="1"/>
-      <c r="V1003" s="1"/>
-      <c r="W1003" s="1"/>
-      <c r="X1003" s="1"/>
-      <c r="Y1003" s="1"/>
-      <c r="Z1003" s="1"/>
-      <c r="AA1003" s="1"/>
-      <c r="AB1003" s="1"/>
-      <c r="AC1003" s="1"/>
-      <c r="AD1003" s="1"/>
-      <c r="AE1003" s="1"/>
-      <c r="AF1003" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="G2:K4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:D5">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C9:C16 C18:C24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C8:C15 C17:C23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J9:J16 J18:J24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J8:J15 J17:J23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Assigned,Started,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated Documents Names and added Block diagrams folder Signed-off-by: Ahmed-Zoher <59732468+Ahmed-Zoher@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEF645B-9921-4BD4-A41F-E727883092FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E2DFB-9A70-45CA-8D2F-739EC3739300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>SIQ Documents Review</t>
+  </si>
+  <si>
+    <t>Week 3</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -323,11 +326,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -598,8 +602,8 @@
   <dimension ref="A1:AF1002"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -665,11 +669,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -704,11 +708,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="31"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -738,11 +742,11 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="33"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -905,7 +909,7 @@
       <c r="H8" s="19">
         <v>43854</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <v>3</v>
       </c>
       <c r="J8" s="16" t="s">
@@ -957,7 +961,7 @@
       <c r="H9" s="19">
         <v>43855</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <v>3</v>
       </c>
       <c r="J9" s="16" t="s">
@@ -1009,7 +1013,7 @@
       <c r="H10" s="19">
         <v>43854</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="22">
         <v>2</v>
       </c>
       <c r="J10" s="16" t="s">
@@ -1061,7 +1065,7 @@
       <c r="H11" s="19">
         <v>43856</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="22">
         <v>2</v>
       </c>
       <c r="J11" s="16" t="s">
@@ -1113,7 +1117,7 @@
       <c r="H12" s="19">
         <v>43855</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="22">
         <v>1</v>
       </c>
       <c r="J12" s="17" t="s">
@@ -1165,7 +1169,7 @@
       <c r="H13" s="19">
         <v>43855</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="22">
         <v>1</v>
       </c>
       <c r="J13" s="17" t="s">
@@ -1217,7 +1221,7 @@
       <c r="H14" s="19">
         <v>43855</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="22">
         <v>1</v>
       </c>
       <c r="J14" s="17" t="s">
@@ -1246,8 +1250,8 @@
       <c r="AE14" s="3"/>
       <c r="AF14" s="5"/>
     </row>
-    <row r="15" spans="1:32" s="25" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+    <row r="15" spans="1:32" s="24" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
       <c r="B15" s="17" t="s">
         <v>29</v>
       </c>
@@ -1269,7 +1273,7 @@
       <c r="H15" s="19">
         <v>43862</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="22">
         <v>3</v>
       </c>
       <c r="J15" s="17" t="s">
@@ -1298,8 +1302,8 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="5"/>
     </row>
-    <row r="16" spans="1:32" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+    <row r="16" spans="1:32" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
       <c r="B16" s="14" t="s">
         <v>32</v>
       </c>
@@ -1334,8 +1338,8 @@
       <c r="AE16" s="3"/>
       <c r="AF16" s="5"/>
     </row>
-    <row r="17" spans="1:32" s="27" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+    <row r="17" spans="1:32" s="26" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
       <c r="B17" s="17" t="s">
         <v>22</v>
       </c>
@@ -1353,7 +1357,7 @@
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
-      <c r="I17" s="23"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="17" t="s">
         <v>30</v>
       </c>
@@ -1380,8 +1384,8 @@
       <c r="AE17" s="3"/>
       <c r="AF17" s="5"/>
     </row>
-    <row r="18" spans="1:32" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+    <row r="18" spans="1:32" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
       <c r="B18" s="17" t="s">
         <v>23</v>
       </c>
@@ -1399,7 +1403,7 @@
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
-      <c r="I18" s="23"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="17" t="s">
         <v>30</v>
       </c>
@@ -1426,8 +1430,8 @@
       <c r="AE18" s="3"/>
       <c r="AF18" s="5"/>
     </row>
-    <row r="19" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+    <row r="19" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
       <c r="B19" s="17" t="s">
         <v>24</v>
       </c>
@@ -1441,11 +1445,11 @@
         <v>43865</v>
       </c>
       <c r="F19" s="19">
-        <v>43835</v>
+        <v>43866</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
-      <c r="I19" s="23"/>
+      <c r="I19" s="22"/>
       <c r="J19" s="17" t="s">
         <v>30</v>
       </c>
@@ -1472,8 +1476,8 @@
       <c r="AE19" s="3"/>
       <c r="AF19" s="5"/>
     </row>
-    <row r="20" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+    <row r="20" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
       <c r="B20" s="17" t="s">
         <v>24</v>
       </c>
@@ -1491,7 +1495,7 @@
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
-      <c r="I20" s="23"/>
+      <c r="I20" s="22"/>
       <c r="J20" s="17" t="s">
         <v>30</v>
       </c>
@@ -1518,8 +1522,8 @@
       <c r="AE20" s="3"/>
       <c r="AF20" s="5"/>
     </row>
-    <row r="21" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+    <row r="21" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
       <c r="B21" s="17" t="s">
         <v>24</v>
       </c>
@@ -1537,7 +1541,7 @@
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
-      <c r="I21" s="23"/>
+      <c r="I21" s="22"/>
       <c r="J21" s="17" t="s">
         <v>30</v>
       </c>
@@ -1564,8 +1568,8 @@
       <c r="AE21" s="3"/>
       <c r="AF21" s="5"/>
     </row>
-    <row r="22" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+    <row r="22" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
       <c r="B22" s="17" t="s">
         <v>34</v>
       </c>
@@ -1583,7 +1587,7 @@
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
-      <c r="I22" s="23"/>
+      <c r="I22" s="22"/>
       <c r="J22" s="17" t="s">
         <v>30</v>
       </c>
@@ -1610,8 +1614,8 @@
       <c r="AE22" s="3"/>
       <c r="AF22" s="5"/>
     </row>
-    <row r="23" spans="1:32" s="27" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:32" s="26" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
       <c r="B23" s="17" t="s">
         <v>35</v>
       </c>
@@ -1629,7 +1633,7 @@
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
-      <c r="I23" s="23"/>
+      <c r="I23" s="22"/>
       <c r="J23" s="17" t="s">
         <v>30</v>
       </c>
@@ -1656,18 +1660,20 @@
       <c r="AE23" s="3"/>
       <c r="AF23" s="5"/>
     </row>
-    <row r="24" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+    <row r="24" spans="1:32" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -1694,7 +1700,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
-      <c r="D25" s="22"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>

</xml_diff>

<commit_message>
Final Cross Review for HSI and CYRS Updated Project Plan Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E2DFB-9A70-45CA-8D2F-739EC3739300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D68B1F-F14F-4461-8277-36A1739C6724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>TASK NAME</t>
-  </si>
-  <si>
-    <t>FEATURE TYPE</t>
   </si>
   <si>
     <t>RESPONSIBLE</t>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>CYRS Documentation</t>
-  </si>
-  <si>
-    <t>Non-Technical</t>
   </si>
   <si>
     <t>SRS Documentation</t>
@@ -129,13 +123,25 @@
     <t>Salma Amr</t>
   </si>
   <si>
-    <t>Overall Documents Review</t>
+    <t>Week 3</t>
   </si>
   <si>
-    <t>SIQ Documents Review</t>
+    <t>HSI Document update</t>
   </si>
   <si>
-    <t>Week 3</t>
+    <t>CYRS Document update</t>
+  </si>
+  <si>
+    <t>SRS Document update</t>
+  </si>
+  <si>
+    <t>SRS Document Review and update</t>
+  </si>
+  <si>
+    <t>Overall Documents Cross Review</t>
+  </si>
+  <si>
+    <t>SIQ Document Update</t>
   </si>
 </sst>
 </file>
@@ -603,20 +609,21 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.36328125" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" customWidth="1"/>
     <col min="3" max="3" width="19.81640625" customWidth="1"/>
     <col min="4" max="4" width="24.1796875" customWidth="1"/>
-    <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1"/>
     <col min="8" max="8" width="15.6328125" customWidth="1"/>
     <col min="9" max="9" width="12.81640625" customWidth="1"/>
-    <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="10" max="10" width="9.08984375" customWidth="1"/>
     <col min="11" max="11" width="50.453125" customWidth="1"/>
     <col min="12" max="12" width="3.36328125" customWidth="1"/>
     <col min="13" max="32" width="11" customWidth="1"/>
@@ -825,9 +832,7 @@
       <c r="J6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -847,23 +852,22 @@
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="5"/>
+      <c r="AE6" s="5"/>
     </row>
     <row r="7" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -883,39 +887,36 @@
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="5"/>
+      <c r="AE7" s="5"/>
     </row>
     <row r="8" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>16</v>
+      <c r="C8" s="17" t="s">
+        <v>18</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="18">
+      <c r="D8" s="18">
         <v>43851</v>
       </c>
+      <c r="E8" s="19">
+        <v>43852</v>
+      </c>
       <c r="F8" s="19">
-        <v>43852</v>
+        <v>43854</v>
       </c>
       <c r="G8" s="19">
         <v>43854</v>
       </c>
-      <c r="H8" s="19">
-        <v>43854</v>
-      </c>
-      <c r="I8" s="22">
+      <c r="H8" s="22">
         <v>3</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>21</v>
+      <c r="I8" s="16" t="s">
+        <v>19</v>
       </c>
-      <c r="K8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -935,39 +936,36 @@
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="5"/>
+      <c r="AE8" s="5"/>
     </row>
     <row r="9" spans="1:32" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>27</v>
+      <c r="D9" s="18">
+        <v>43852</v>
       </c>
-      <c r="E9" s="18">
-        <v>43852</v>
+      <c r="E9" s="19">
+        <v>43854</v>
       </c>
       <c r="F9" s="19">
         <v>43854</v>
       </c>
       <c r="G9" s="19">
-        <v>43854</v>
-      </c>
-      <c r="H9" s="19">
         <v>43855</v>
       </c>
-      <c r="I9" s="22">
+      <c r="H9" s="22">
         <v>3</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>21</v>
+      <c r="I9" s="16" t="s">
+        <v>19</v>
       </c>
-      <c r="K9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -987,22 +985,21 @@
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="5"/>
+      <c r="AE9" s="5"/>
     </row>
     <row r="10" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>16</v>
+      <c r="C10" s="17" t="s">
+        <v>26</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>28</v>
+      <c r="D10" s="18">
+        <v>43852</v>
       </c>
-      <c r="E10" s="18">
-        <v>43852</v>
+      <c r="E10" s="19">
+        <v>43854</v>
       </c>
       <c r="F10" s="19">
         <v>43854</v>
@@ -1010,16 +1007,14 @@
       <c r="G10" s="19">
         <v>43854</v>
       </c>
-      <c r="H10" s="19">
-        <v>43854</v>
-      </c>
-      <c r="I10" s="22">
+      <c r="H10" s="22">
         <v>2</v>
       </c>
-      <c r="J10" s="16" t="s">
-        <v>21</v>
+      <c r="I10" s="16" t="s">
+        <v>19</v>
       </c>
-      <c r="K10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -1039,39 +1034,36 @@
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="5"/>
+      <c r="AE10" s="5"/>
     </row>
     <row r="11" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>25</v>
+      <c r="C11" s="17" t="s">
+        <v>23</v>
       </c>
-      <c r="E11" s="18">
+      <c r="D11" s="18">
         <v>43852</v>
       </c>
-      <c r="F11" s="19">
+      <c r="E11" s="19">
         <v>43854</v>
       </c>
-      <c r="G11" s="19">
+      <c r="F11" s="19">
         <v>43855</v>
       </c>
-      <c r="H11" s="19">
+      <c r="G11" s="19">
         <v>43856</v>
       </c>
-      <c r="I11" s="22">
+      <c r="H11" s="22">
         <v>2</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>21</v>
+      <c r="I11" s="16" t="s">
+        <v>19</v>
       </c>
-      <c r="K11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -1091,39 +1083,36 @@
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="5"/>
+      <c r="AE11" s="5"/>
     </row>
     <row r="12" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="19">
+      <c r="D12" s="19">
         <v>43855</v>
       </c>
+      <c r="E12" s="19">
+        <v>43856</v>
+      </c>
       <c r="F12" s="19">
-        <v>43856</v>
+        <v>43855</v>
       </c>
       <c r="G12" s="19">
         <v>43855</v>
       </c>
-      <c r="H12" s="19">
-        <v>43855</v>
-      </c>
-      <c r="I12" s="22">
+      <c r="H12" s="22">
         <v>1</v>
       </c>
-      <c r="J12" s="17" t="s">
-        <v>21</v>
+      <c r="I12" s="17" t="s">
+        <v>19</v>
       </c>
-      <c r="K12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -1143,39 +1132,36 @@
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
-      <c r="AE12" s="3"/>
-      <c r="AF12" s="5"/>
+      <c r="AE12" s="5"/>
     </row>
     <row r="13" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="19">
+      <c r="D13" s="19">
         <v>43854</v>
       </c>
-      <c r="F13" s="19">
+      <c r="E13" s="19">
         <v>43855</v>
       </c>
-      <c r="G13" s="19">
+      <c r="F13" s="19">
         <v>43854</v>
       </c>
-      <c r="H13" s="19">
+      <c r="G13" s="19">
         <v>43855</v>
       </c>
-      <c r="I13" s="22">
+      <c r="H13" s="22">
         <v>1</v>
       </c>
-      <c r="J13" s="17" t="s">
-        <v>21</v>
+      <c r="I13" s="17" t="s">
+        <v>19</v>
       </c>
-      <c r="K13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -1195,39 +1181,36 @@
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="5"/>
+      <c r="AE13" s="5"/>
     </row>
     <row r="14" spans="1:32" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>26</v>
+      <c r="D14" s="19">
+        <v>43855</v>
       </c>
       <c r="E14" s="19">
-        <v>43855</v>
+        <v>43856</v>
       </c>
       <c r="F14" s="19">
-        <v>43856</v>
+        <v>43855</v>
       </c>
       <c r="G14" s="19">
         <v>43855</v>
       </c>
-      <c r="H14" s="19">
-        <v>43855</v>
-      </c>
-      <c r="I14" s="22">
+      <c r="H14" s="22">
         <v>1</v>
       </c>
-      <c r="J14" s="17" t="s">
-        <v>21</v>
+      <c r="I14" s="17" t="s">
+        <v>19</v>
       </c>
-      <c r="K14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -1247,39 +1230,36 @@
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="5"/>
+      <c r="AE14" s="5"/>
     </row>
     <row r="15" spans="1:32" s="24" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>26</v>
+      <c r="D15" s="19">
+        <v>43858</v>
       </c>
       <c r="E15" s="19">
+        <v>43860</v>
+      </c>
+      <c r="F15" s="19">
         <v>43858</v>
       </c>
-      <c r="F15" s="19">
-        <v>43860</v>
-      </c>
       <c r="G15" s="19">
-        <v>43858</v>
-      </c>
-      <c r="H15" s="19">
         <v>43862</v>
       </c>
-      <c r="I15" s="22">
+      <c r="H15" s="22">
         <v>3</v>
       </c>
-      <c r="J15" s="17" t="s">
-        <v>21</v>
+      <c r="I15" s="17" t="s">
+        <v>19</v>
       </c>
-      <c r="K15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -1299,23 +1279,22 @@
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="5"/>
+      <c r="AE15" s="5"/>
     </row>
     <row r="16" spans="1:32" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
+      <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -1335,33 +1314,36 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="5"/>
+      <c r="AE16" s="5"/>
     </row>
     <row r="17" spans="1:32" s="26" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="17" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>28</v>
+      <c r="D17" s="19">
+        <v>43863</v>
       </c>
       <c r="E17" s="19">
-        <v>43863</v>
+        <v>43864</v>
       </c>
       <c r="F17" s="19">
         <v>43864</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="17" t="s">
-        <v>30</v>
+      <c r="G17" s="19">
+        <v>43864</v>
       </c>
-      <c r="K17" s="17"/>
+      <c r="H17" s="22">
+        <v>1</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -1381,33 +1363,36 @@
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="5"/>
+      <c r="AE17" s="5"/>
     </row>
     <row r="18" spans="1:32" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="17" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>33</v>
+      <c r="D18" s="19">
+        <v>43863</v>
       </c>
       <c r="E18" s="19">
+        <v>43864</v>
+      </c>
+      <c r="F18" s="19">
         <v>43863</v>
       </c>
-      <c r="F18" s="19">
+      <c r="G18" s="19">
         <v>43864</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="17" t="s">
-        <v>30</v>
+      <c r="H18" s="22">
+        <v>2</v>
       </c>
-      <c r="K18" s="17"/>
+      <c r="I18" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1427,33 +1412,36 @@
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="5"/>
+      <c r="AE18" s="5"/>
     </row>
     <row r="19" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
       <c r="B19" s="17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>27</v>
+      <c r="D19" s="19">
+        <v>43865</v>
       </c>
       <c r="E19" s="19">
-        <v>43865</v>
+        <v>43866</v>
       </c>
       <c r="F19" s="19">
         <v>43866</v>
       </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="17" t="s">
-        <v>30</v>
+      <c r="G19" s="19">
+        <v>43866</v>
       </c>
-      <c r="K19" s="17"/>
+      <c r="H19" s="22">
+        <v>1</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -1473,33 +1461,36 @@
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="5"/>
+      <c r="AE19" s="5"/>
     </row>
     <row r="20" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="17" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>25</v>
+      <c r="D20" s="19">
+        <v>43866</v>
       </c>
       <c r="E20" s="19">
-        <v>43866</v>
+        <v>43867</v>
       </c>
       <c r="F20" s="19">
         <v>43867</v>
       </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="17" t="s">
-        <v>30</v>
+      <c r="G20" s="19">
+        <v>43867</v>
       </c>
-      <c r="K20" s="17"/>
+      <c r="H20" s="22">
+        <v>1</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -1519,33 +1510,30 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="5"/>
+      <c r="AE20" s="5"/>
     </row>
     <row r="21" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="17" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>20</v>
+      <c r="D21" s="19">
+        <v>43867</v>
       </c>
       <c r="E21" s="19">
-        <v>43867</v>
-      </c>
-      <c r="F21" s="19">
         <v>43868</v>
       </c>
+      <c r="F21" s="19"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="17" t="s">
-        <v>30</v>
+      <c r="H21" s="22"/>
+      <c r="I21" s="17" t="s">
+        <v>28</v>
       </c>
-      <c r="K21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -1565,33 +1553,30 @@
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="5"/>
+      <c r="AE21" s="5"/>
     </row>
     <row r="22" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="19">
+      <c r="D22" s="19">
         <v>43868</v>
       </c>
-      <c r="F22" s="19">
+      <c r="E22" s="19">
         <v>43869</v>
       </c>
+      <c r="F22" s="19"/>
       <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="17" t="s">
-        <v>30</v>
+      <c r="H22" s="22"/>
+      <c r="I22" s="17" t="s">
+        <v>28</v>
       </c>
-      <c r="K22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -1611,33 +1596,30 @@
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="5"/>
+      <c r="AE22" s="5"/>
     </row>
     <row r="23" spans="1:32" s="26" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="19">
+      <c r="D23" s="19">
         <v>43868</v>
       </c>
-      <c r="F23" s="19">
+      <c r="E23" s="19">
         <v>43869</v>
       </c>
+      <c r="F23" s="19"/>
       <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="17" t="s">
-        <v>30</v>
+      <c r="H23" s="22"/>
+      <c r="I23" s="17" t="s">
+        <v>28</v>
       </c>
-      <c r="K23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -1657,23 +1639,22 @@
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
-      <c r="AE23" s="3"/>
-      <c r="AF23" s="5"/>
+      <c r="AE23" s="5"/>
     </row>
     <row r="24" spans="1:32" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
+      <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -1693,8 +1674,7 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
-      <c r="AE24" s="3"/>
-      <c r="AF24" s="5"/>
+      <c r="AE24" s="5"/>
     </row>
     <row r="25" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -34952,11 +34932,8 @@
   <mergeCells count="1">
     <mergeCell ref="G2:K4"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C8:C15 C17:C23" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Technical,Non-Technical"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J8:J15 J17:J23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Assigned,Started,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated project plan Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D68B1F-F14F-4461-8277-36A1739C6724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF73193-1849-4642-8268-7715A75B33DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -138,10 +138,13 @@
     <t>SRS Document Review and update</t>
   </si>
   <si>
-    <t>Overall Documents Cross Review</t>
+    <t>SIQ Document Update</t>
   </si>
   <si>
-    <t>SIQ Document Update</t>
+    <t>CYRS and HIS Final Cross Review</t>
+  </si>
+  <si>
+    <t>SRS Final Cross Review</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -336,6 +339,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -605,11 +610,11 @@
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF1002"/>
+  <dimension ref="A1:AF1003"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -676,11 +681,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="33"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -715,11 +720,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="33"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -749,11 +754,11 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="35"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -1555,10 +1560,10 @@
       <c r="AD21" s="3"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+    <row r="22" spans="1:32" s="30" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
       <c r="B22" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>4</v>
@@ -1569,11 +1574,17 @@
       <c r="E22" s="19">
         <v>43869</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="22"/>
+      <c r="F22" s="19">
+        <v>43868</v>
+      </c>
+      <c r="G22" s="19">
+        <v>43868</v>
+      </c>
+      <c r="H22" s="22">
+        <v>1</v>
+      </c>
       <c r="I22" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="3"/>
@@ -1598,10 +1609,10 @@
       <c r="AD22" s="3"/>
       <c r="AE22" s="5"/>
     </row>
-    <row r="23" spans="1:32" s="26" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>4</v>
@@ -1641,19 +1652,33 @@
       <c r="AD23" s="3"/>
       <c r="AE23" s="5"/>
     </row>
-    <row r="24" spans="1:32" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="14" t="s">
-        <v>32</v>
+    <row r="24" spans="1:32" s="26" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="17" t="s">
+        <v>37</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="C24" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="19">
+        <v>43868</v>
+      </c>
+      <c r="E24" s="19">
+        <v>43869</v>
+      </c>
+      <c r="F24" s="19">
+        <v>43868</v>
+      </c>
+      <c r="G24" s="19">
+        <v>43869</v>
+      </c>
+      <c r="H24" s="22">
+        <v>2</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="17"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1676,17 +1701,19 @@
       <c r="AD24" s="3"/>
       <c r="AE24" s="5"/>
     </row>
-    <row r="25" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+    <row r="25" spans="1:32" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
+      <c r="B25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1707,14 +1734,13 @@
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
-      <c r="AE25" s="3"/>
-      <c r="AF25" s="5"/>
+      <c r="AE25" s="5"/>
     </row>
     <row r="26" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -2118,73 +2144,73 @@
       <c r="AE37" s="3"/>
       <c r="AF37" s="5"/>
     </row>
-    <row r="38" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
-    </row>
-    <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="5"/>
+    </row>
+    <row r="39" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AA39" s="3"/>
-      <c r="AB39" s="3"/>
-      <c r="AC39" s="3"/>
-      <c r="AD39" s="3"/>
-      <c r="AE39" s="3"/>
-      <c r="AF39" s="5"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
     </row>
     <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -8410,37 +8436,37 @@
     </row>
     <row r="223" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
-      <c r="D223" s="1"/>
-      <c r="E223" s="1"/>
-      <c r="F223" s="1"/>
-      <c r="G223" s="1"/>
-      <c r="H223" s="1"/>
-      <c r="I223" s="1"/>
-      <c r="J223" s="1"/>
-      <c r="K223" s="1"/>
-      <c r="L223" s="1"/>
-      <c r="M223" s="1"/>
-      <c r="N223" s="1"/>
-      <c r="O223" s="1"/>
-      <c r="P223" s="1"/>
-      <c r="Q223" s="1"/>
-      <c r="R223" s="1"/>
-      <c r="S223" s="1"/>
-      <c r="T223" s="1"/>
-      <c r="U223" s="1"/>
-      <c r="V223" s="1"/>
-      <c r="W223" s="1"/>
-      <c r="X223" s="1"/>
-      <c r="Y223" s="1"/>
-      <c r="Z223" s="1"/>
-      <c r="AA223" s="1"/>
-      <c r="AB223" s="1"/>
-      <c r="AC223" s="1"/>
-      <c r="AD223" s="1"/>
-      <c r="AE223" s="1"/>
-      <c r="AF223" s="1"/>
+      <c r="B223" s="3"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="3"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
+      <c r="H223" s="3"/>
+      <c r="I223" s="3"/>
+      <c r="J223" s="3"/>
+      <c r="K223" s="3"/>
+      <c r="L223" s="3"/>
+      <c r="M223" s="3"/>
+      <c r="N223" s="3"/>
+      <c r="O223" s="3"/>
+      <c r="P223" s="3"/>
+      <c r="Q223" s="3"/>
+      <c r="R223" s="3"/>
+      <c r="S223" s="3"/>
+      <c r="T223" s="3"/>
+      <c r="U223" s="3"/>
+      <c r="V223" s="3"/>
+      <c r="W223" s="3"/>
+      <c r="X223" s="3"/>
+      <c r="Y223" s="3"/>
+      <c r="Z223" s="3"/>
+      <c r="AA223" s="3"/>
+      <c r="AB223" s="3"/>
+      <c r="AC223" s="3"/>
+      <c r="AD223" s="3"/>
+      <c r="AE223" s="3"/>
+      <c r="AF223" s="5"/>
     </row>
     <row r="224" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
@@ -34928,12 +34954,46 @@
       <c r="AE1002" s="1"/>
       <c r="AF1002" s="1"/>
     </row>
+    <row r="1003" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+      <c r="AA1003" s="1"/>
+      <c r="AB1003" s="1"/>
+      <c r="AC1003" s="1"/>
+      <c r="AD1003" s="1"/>
+      <c r="AE1003" s="1"/>
+      <c r="AF1003" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G2:K4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Assigned,Started,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated Project Plan: adding week 3 tasks. Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F41E52-F828-4A55-9F1C-9D8113E8F2DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF22AD09-96CF-4095-AE39-5DECCD543AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -146,6 +146,24 @@
   <si>
     <t>SRS Final Cross Review</t>
   </si>
+  <si>
+    <t xml:space="preserve">HSI Final Update and Review acording to the session's feedback </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYRS Final Update and Review acording to the session's feedback </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS Update according to session's review and review excel sheet </t>
+  </si>
+  <si>
+    <t>SRS cross review and update</t>
+  </si>
+  <si>
+    <t>RTM review and update according to finalized SRS, HSI and CYRS</t>
+  </si>
+  <si>
+    <t>RTM cross review and update</t>
+  </si>
 </sst>
 </file>
 
@@ -154,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -190,12 +208,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Century Gothic"/>
     </font>
   </fonts>
   <fills count="6">
@@ -334,8 +346,6 @@
     <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -345,12 +355,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,8 +624,8 @@
   <dimension ref="A1:AF1003"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD25"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -680,11 +692,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -719,11 +731,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -753,11 +765,11 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -913,7 +925,7 @@
       <c r="G8" s="19">
         <v>43854</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="20">
         <v>3</v>
       </c>
       <c r="I8" s="16" t="s">
@@ -962,7 +974,7 @@
       <c r="G9" s="19">
         <v>43855</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="20">
         <v>3</v>
       </c>
       <c r="I9" s="16" t="s">
@@ -1011,7 +1023,7 @@
       <c r="G10" s="19">
         <v>43854</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="20">
         <v>2</v>
       </c>
       <c r="I10" s="16" t="s">
@@ -1060,7 +1072,7 @@
       <c r="G11" s="19">
         <v>43856</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="20">
         <v>2</v>
       </c>
       <c r="I11" s="16" t="s">
@@ -1109,7 +1121,7 @@
       <c r="G12" s="19">
         <v>43855</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="20">
         <v>1</v>
       </c>
       <c r="I12" s="17" t="s">
@@ -1158,7 +1170,7 @@
       <c r="G13" s="19">
         <v>43855</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="20">
         <v>1</v>
       </c>
       <c r="I13" s="17" t="s">
@@ -1207,7 +1219,7 @@
       <c r="G14" s="19">
         <v>43855</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="20">
         <v>1</v>
       </c>
       <c r="I14" s="17" t="s">
@@ -1236,8 +1248,8 @@
       <c r="AD14" s="3"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:32" s="24" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+    <row r="15" spans="1:32" s="22" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
       <c r="B15" s="17" t="s">
         <v>27</v>
       </c>
@@ -1256,7 +1268,7 @@
       <c r="G15" s="19">
         <v>43862</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="20">
         <v>3</v>
       </c>
       <c r="I15" s="17" t="s">
@@ -1285,8 +1297,8 @@
       <c r="AD15" s="3"/>
       <c r="AE15" s="5"/>
     </row>
-    <row r="16" spans="1:32" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+    <row r="16" spans="1:32" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
       <c r="B16" s="14" t="s">
         <v>30</v>
       </c>
@@ -1320,8 +1332,8 @@
       <c r="AD16" s="3"/>
       <c r="AE16" s="5"/>
     </row>
-    <row r="17" spans="1:32" s="26" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+    <row r="17" spans="1:32" s="24" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
       <c r="B17" s="17" t="s">
         <v>33</v>
       </c>
@@ -1340,7 +1352,7 @@
       <c r="G17" s="19">
         <v>43864</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="20">
         <v>1</v>
       </c>
       <c r="I17" s="17" t="s">
@@ -1369,8 +1381,8 @@
       <c r="AD17" s="3"/>
       <c r="AE17" s="5"/>
     </row>
-    <row r="18" spans="1:32" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+    <row r="18" spans="1:32" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
       <c r="B18" s="17" t="s">
         <v>34</v>
       </c>
@@ -1389,7 +1401,7 @@
       <c r="G18" s="19">
         <v>43864</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="20">
         <v>2</v>
       </c>
       <c r="I18" s="17" t="s">
@@ -1418,8 +1430,8 @@
       <c r="AD18" s="3"/>
       <c r="AE18" s="5"/>
     </row>
-    <row r="19" spans="1:32" s="26" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+    <row r="19" spans="1:32" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
       <c r="B19" s="17" t="s">
         <v>35</v>
       </c>
@@ -1438,7 +1450,7 @@
       <c r="G19" s="19">
         <v>43866</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="20">
         <v>1</v>
       </c>
       <c r="I19" s="17" t="s">
@@ -1467,8 +1479,8 @@
       <c r="AD19" s="3"/>
       <c r="AE19" s="5"/>
     </row>
-    <row r="20" spans="1:32" s="34" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+    <row r="20" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
       <c r="B20" s="17" t="s">
         <v>36</v>
       </c>
@@ -1487,37 +1499,37 @@
       <c r="G20" s="19">
         <v>43867</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="20">
         <v>1</v>
       </c>
       <c r="I20" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="17"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="33"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="33"/>
-      <c r="AB20" s="33"/>
-      <c r="AC20" s="33"/>
-      <c r="AD20" s="33"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="27"/>
+      <c r="AC20" s="27"/>
+      <c r="AD20" s="27"/>
       <c r="AE20" s="5"/>
     </row>
-    <row r="21" spans="1:32" s="34" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+    <row r="21" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
       <c r="B21" s="17" t="s">
         <v>36</v>
       </c>
@@ -1532,35 +1544,35 @@
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J21" s="17"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="33"/>
-      <c r="V21" s="33"/>
-      <c r="W21" s="33"/>
-      <c r="X21" s="33"/>
-      <c r="Y21" s="33"/>
-      <c r="Z21" s="33"/>
-      <c r="AA21" s="33"/>
-      <c r="AB21" s="33"/>
-      <c r="AC21" s="33"/>
-      <c r="AD21" s="33"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="27"/>
+      <c r="AC21" s="27"/>
+      <c r="AD21" s="27"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:32" s="34" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+    <row r="22" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
       <c r="B22" s="17" t="s">
         <v>39</v>
       </c>
@@ -1575,35 +1587,35 @@
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
-      <c r="H22" s="22"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J22" s="17"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="33"/>
-      <c r="V22" s="33"/>
-      <c r="W22" s="33"/>
-      <c r="X22" s="33"/>
-      <c r="Y22" s="33"/>
-      <c r="Z22" s="33"/>
-      <c r="AA22" s="33"/>
-      <c r="AB22" s="33"/>
-      <c r="AC22" s="33"/>
-      <c r="AD22" s="33"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="27"/>
+      <c r="AC22" s="27"/>
+      <c r="AD22" s="27"/>
       <c r="AE22" s="5"/>
     </row>
-    <row r="23" spans="1:32" s="34" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+    <row r="23" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
       <c r="B23" s="17" t="s">
         <v>38</v>
       </c>
@@ -1622,37 +1634,37 @@
       <c r="G23" s="19">
         <v>43868</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="20">
         <v>1</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="17"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="33"/>
-      <c r="S23" s="33"/>
-      <c r="T23" s="33"/>
-      <c r="U23" s="33"/>
-      <c r="V23" s="33"/>
-      <c r="W23" s="33"/>
-      <c r="X23" s="33"/>
-      <c r="Y23" s="33"/>
-      <c r="Z23" s="33"/>
-      <c r="AA23" s="33"/>
-      <c r="AB23" s="33"/>
-      <c r="AC23" s="33"/>
-      <c r="AD23" s="33"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="27"/>
+      <c r="AB23" s="27"/>
+      <c r="AC23" s="27"/>
+      <c r="AD23" s="27"/>
       <c r="AE23" s="5"/>
     </row>
-    <row r="24" spans="1:32" s="34" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+    <row r="24" spans="1:32" s="28" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
       <c r="B24" s="17" t="s">
         <v>37</v>
       </c>
@@ -1671,37 +1683,37 @@
       <c r="G24" s="19">
         <v>43869</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="20">
         <v>1</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J24" s="17"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="33"/>
-      <c r="W24" s="33"/>
-      <c r="X24" s="33"/>
-      <c r="Y24" s="33"/>
-      <c r="Z24" s="33"/>
-      <c r="AA24" s="33"/>
-      <c r="AB24" s="33"/>
-      <c r="AC24" s="33"/>
-      <c r="AD24" s="33"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
+      <c r="AA24" s="27"/>
+      <c r="AB24" s="27"/>
+      <c r="AC24" s="27"/>
+      <c r="AD24" s="27"/>
       <c r="AE24" s="5"/>
     </row>
-    <row r="25" spans="1:32" s="34" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+    <row r="25" spans="1:32" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
       <c r="B25" s="14" t="s">
         <v>32</v>
       </c>
@@ -1713,231 +1725,285 @@
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="33"/>
-      <c r="W25" s="33"/>
-      <c r="X25" s="33"/>
-      <c r="Y25" s="33"/>
-      <c r="Z25" s="33"/>
-      <c r="AA25" s="33"/>
-      <c r="AB25" s="33"/>
-      <c r="AC25" s="33"/>
-      <c r="AD25" s="33"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27"/>
+      <c r="AA25" s="27"/>
+      <c r="AB25" s="27"/>
+      <c r="AC25" s="27"/>
+      <c r="AD25" s="27"/>
       <c r="AE25" s="5"/>
     </row>
-    <row r="26" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="5"/>
-    </row>
-    <row r="27" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-      <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
-      <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
-      <c r="Z27" s="3"/>
-      <c r="AA27" s="3"/>
-      <c r="AB27" s="3"/>
-      <c r="AC27" s="3"/>
-      <c r="AD27" s="3"/>
-      <c r="AE27" s="3"/>
-      <c r="AF27" s="5"/>
-    </row>
-    <row r="28" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
-      <c r="AA28" s="3"/>
-      <c r="AB28" s="3"/>
-      <c r="AC28" s="3"/>
-      <c r="AD28" s="3"/>
-      <c r="AE28" s="3"/>
-      <c r="AF28" s="5"/>
-    </row>
-    <row r="29" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
-      <c r="AC29" s="3"/>
-      <c r="AD29" s="3"/>
-      <c r="AE29" s="3"/>
-      <c r="AF29" s="5"/>
-    </row>
-    <row r="30" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AA30" s="3"/>
-      <c r="AB30" s="3"/>
-      <c r="AC30" s="3"/>
-      <c r="AD30" s="3"/>
-      <c r="AE30" s="3"/>
-      <c r="AF30" s="5"/>
-    </row>
-    <row r="31" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
-      <c r="AB31" s="3"/>
-      <c r="AC31" s="3"/>
-      <c r="AD31" s="3"/>
-      <c r="AE31" s="3"/>
-      <c r="AF31" s="5"/>
+    <row r="26" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="19">
+        <v>43869</v>
+      </c>
+      <c r="E26" s="19">
+        <v>43869</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="17"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="27"/>
+      <c r="AA26" s="27"/>
+      <c r="AB26" s="27"/>
+      <c r="AC26" s="27"/>
+      <c r="AD26" s="27"/>
+      <c r="AE26" s="5"/>
+    </row>
+    <row r="27" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="19">
+        <v>43869</v>
+      </c>
+      <c r="E27" s="19">
+        <v>43869</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="17"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
+      <c r="V27" s="27"/>
+      <c r="W27" s="27"/>
+      <c r="X27" s="27"/>
+      <c r="Y27" s="27"/>
+      <c r="Z27" s="27"/>
+      <c r="AA27" s="27"/>
+      <c r="AB27" s="27"/>
+      <c r="AC27" s="27"/>
+      <c r="AD27" s="27"/>
+      <c r="AE27" s="5"/>
+    </row>
+    <row r="28" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="19">
+        <v>43870</v>
+      </c>
+      <c r="E28" s="19">
+        <v>43872</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="17"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="27"/>
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="27"/>
+      <c r="V28" s="27"/>
+      <c r="W28" s="27"/>
+      <c r="X28" s="27"/>
+      <c r="Y28" s="27"/>
+      <c r="Z28" s="27"/>
+      <c r="AA28" s="27"/>
+      <c r="AB28" s="27"/>
+      <c r="AC28" s="27"/>
+      <c r="AD28" s="27"/>
+      <c r="AE28" s="5"/>
+    </row>
+    <row r="29" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="19">
+        <v>43872</v>
+      </c>
+      <c r="E29" s="19">
+        <v>43873</v>
+      </c>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="27"/>
+      <c r="Z29" s="27"/>
+      <c r="AA29" s="27"/>
+      <c r="AB29" s="27"/>
+      <c r="AC29" s="27"/>
+      <c r="AD29" s="27"/>
+      <c r="AE29" s="5"/>
+    </row>
+    <row r="30" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
+      <c r="B30" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="19">
+        <v>43873</v>
+      </c>
+      <c r="E30" s="19">
+        <v>43874</v>
+      </c>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="17"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27"/>
+      <c r="V30" s="27"/>
+      <c r="W30" s="27"/>
+      <c r="X30" s="27"/>
+      <c r="Y30" s="27"/>
+      <c r="Z30" s="27"/>
+      <c r="AA30" s="27"/>
+      <c r="AB30" s="27"/>
+      <c r="AC30" s="27"/>
+      <c r="AD30" s="27"/>
+      <c r="AE30" s="5"/>
+    </row>
+    <row r="31" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
+      <c r="B31" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="19">
+        <v>43874</v>
+      </c>
+      <c r="E31" s="19">
+        <v>43874</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="17"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="27"/>
+      <c r="S31" s="27"/>
+      <c r="T31" s="27"/>
+      <c r="U31" s="27"/>
+      <c r="V31" s="27"/>
+      <c r="W31" s="27"/>
+      <c r="X31" s="27"/>
+      <c r="Y31" s="27"/>
+      <c r="Z31" s="27"/>
+      <c r="AA31" s="27"/>
+      <c r="AB31" s="27"/>
+      <c r="AC31" s="27"/>
+      <c r="AD31" s="27"/>
+      <c r="AE31" s="5"/>
     </row>
     <row r="32" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
@@ -34992,7 +35058,7 @@
     <mergeCell ref="G2:K4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I24 I26:I31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Assigned,Started,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Project Plan Updated Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF22AD09-96CF-4095-AE39-5DECCD543AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F59C683-A5E5-475B-92EC-56A9E274810D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,8 +624,8 @@
   <dimension ref="A1:AF1003"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1761,11 +1761,17 @@
       <c r="E26" s="19">
         <v>43869</v>
       </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="20"/>
+      <c r="F26" s="19">
+        <v>43869</v>
+      </c>
+      <c r="G26" s="19">
+        <v>43869</v>
+      </c>
+      <c r="H26" s="20">
+        <v>1</v>
+      </c>
       <c r="I26" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J26" s="17"/>
       <c r="K26" s="27"/>
@@ -1804,11 +1810,17 @@
       <c r="E27" s="19">
         <v>43869</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="20"/>
+      <c r="F27" s="19">
+        <v>43869</v>
+      </c>
+      <c r="G27" s="19">
+        <v>43869</v>
+      </c>
+      <c r="H27" s="20">
+        <v>1</v>
+      </c>
       <c r="I27" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J27" s="17"/>
       <c r="K27" s="27"/>

</xml_diff>

<commit_message>
updated the project plan with the completed tasks Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F59C683-A5E5-475B-92EC-56A9E274810D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913CF577-C61C-4F9D-8589-42F4D374A014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,8 +624,8 @@
   <dimension ref="A1:AF1003"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1859,11 +1859,17 @@
       <c r="E28" s="19">
         <v>43872</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="20"/>
+      <c r="F28" s="19">
+        <v>43870</v>
+      </c>
+      <c r="G28" s="19">
+        <v>43872</v>
+      </c>
+      <c r="H28" s="20">
+        <v>3</v>
+      </c>
       <c r="I28" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J28" s="17"/>
       <c r="K28" s="27"/>

</xml_diff>

<commit_message>
Updated Project Plan with the current progress Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913CF577-C61C-4F9D-8589-42F4D374A014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1C44F4-AB07-4BCE-8642-A34205DF31F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,7 +162,7 @@
     <t>RTM review and update according to finalized SRS, HSI and CYRS</t>
   </si>
   <si>
-    <t>RTM cross review and update</t>
+    <t>RTM and SRS cross review and update</t>
   </si>
 </sst>
 </file>
@@ -621,11 +621,11 @@
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF1003"/>
+  <dimension ref="A1:AF1002"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1908,11 +1908,17 @@
       <c r="E29" s="19">
         <v>43873</v>
       </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="20"/>
+      <c r="F29" s="19">
+        <v>43873</v>
+      </c>
+      <c r="G29" s="19">
+        <v>43873</v>
+      </c>
+      <c r="H29" s="20">
+        <v>1</v>
+      </c>
       <c r="I29" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="27"/>
@@ -1940,13 +1946,13 @@
     <row r="30" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D30" s="19">
-        <v>43873</v>
+        <v>43874</v>
       </c>
       <c r="E30" s="19">
         <v>43874</v>
@@ -1983,13 +1989,13 @@
     <row r="31" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
       <c r="B31" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D31" s="19">
-        <v>43874</v>
+        <v>43873</v>
       </c>
       <c r="E31" s="19">
         <v>43874</v>
@@ -2227,73 +2233,73 @@
       <c r="AE37" s="3"/>
       <c r="AF37" s="5"/>
     </row>
-    <row r="38" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="3"/>
-      <c r="AC38" s="3"/>
-      <c r="AD38" s="3"/>
-      <c r="AE38" s="3"/>
-      <c r="AF38" s="5"/>
-    </row>
-    <row r="39" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+    </row>
+    <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
-      <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-      <c r="AF39" s="1"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="5"/>
     </row>
     <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -8519,37 +8525,37 @@
     </row>
     <row r="223" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
-      <c r="B223" s="3"/>
-      <c r="C223" s="3"/>
-      <c r="D223" s="3"/>
-      <c r="E223" s="3"/>
-      <c r="F223" s="3"/>
-      <c r="G223" s="3"/>
-      <c r="H223" s="3"/>
-      <c r="I223" s="3"/>
-      <c r="J223" s="3"/>
-      <c r="K223" s="3"/>
-      <c r="L223" s="3"/>
-      <c r="M223" s="3"/>
-      <c r="N223" s="3"/>
-      <c r="O223" s="3"/>
-      <c r="P223" s="3"/>
-      <c r="Q223" s="3"/>
-      <c r="R223" s="3"/>
-      <c r="S223" s="3"/>
-      <c r="T223" s="3"/>
-      <c r="U223" s="3"/>
-      <c r="V223" s="3"/>
-      <c r="W223" s="3"/>
-      <c r="X223" s="3"/>
-      <c r="Y223" s="3"/>
-      <c r="Z223" s="3"/>
-      <c r="AA223" s="3"/>
-      <c r="AB223" s="3"/>
-      <c r="AC223" s="3"/>
-      <c r="AD223" s="3"/>
-      <c r="AE223" s="3"/>
-      <c r="AF223" s="5"/>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
+      <c r="D223" s="1"/>
+      <c r="E223" s="1"/>
+      <c r="F223" s="1"/>
+      <c r="G223" s="1"/>
+      <c r="H223" s="1"/>
+      <c r="I223" s="1"/>
+      <c r="J223" s="1"/>
+      <c r="K223" s="1"/>
+      <c r="L223" s="1"/>
+      <c r="M223" s="1"/>
+      <c r="N223" s="1"/>
+      <c r="O223" s="1"/>
+      <c r="P223" s="1"/>
+      <c r="Q223" s="1"/>
+      <c r="R223" s="1"/>
+      <c r="S223" s="1"/>
+      <c r="T223" s="1"/>
+      <c r="U223" s="1"/>
+      <c r="V223" s="1"/>
+      <c r="W223" s="1"/>
+      <c r="X223" s="1"/>
+      <c r="Y223" s="1"/>
+      <c r="Z223" s="1"/>
+      <c r="AA223" s="1"/>
+      <c r="AB223" s="1"/>
+      <c r="AC223" s="1"/>
+      <c r="AD223" s="1"/>
+      <c r="AE223" s="1"/>
+      <c r="AF223" s="1"/>
     </row>
     <row r="224" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
@@ -35037,40 +35043,6 @@
       <c r="AE1002" s="1"/>
       <c r="AF1002" s="1"/>
     </row>
-    <row r="1003" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1003" s="1"/>
-      <c r="B1003" s="1"/>
-      <c r="C1003" s="1"/>
-      <c r="D1003" s="1"/>
-      <c r="E1003" s="1"/>
-      <c r="F1003" s="1"/>
-      <c r="G1003" s="1"/>
-      <c r="H1003" s="1"/>
-      <c r="I1003" s="1"/>
-      <c r="J1003" s="1"/>
-      <c r="K1003" s="1"/>
-      <c r="L1003" s="1"/>
-      <c r="M1003" s="1"/>
-      <c r="N1003" s="1"/>
-      <c r="O1003" s="1"/>
-      <c r="P1003" s="1"/>
-      <c r="Q1003" s="1"/>
-      <c r="R1003" s="1"/>
-      <c r="S1003" s="1"/>
-      <c r="T1003" s="1"/>
-      <c r="U1003" s="1"/>
-      <c r="V1003" s="1"/>
-      <c r="W1003" s="1"/>
-      <c r="X1003" s="1"/>
-      <c r="Y1003" s="1"/>
-      <c r="Z1003" s="1"/>
-      <c r="AA1003" s="1"/>
-      <c r="AB1003" s="1"/>
-      <c r="AC1003" s="1"/>
-      <c r="AD1003" s="1"/>
-      <c r="AE1003" s="1"/>
-      <c r="AF1003" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G2:K4"/>

</xml_diff>

<commit_message>
Updated Project Plan with Current Progress Updated SRS review sheet with the status of the review points Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8A48FE-6BA9-476C-8066-BCB75C18F9A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1972E42-7B23-493C-A4DF-91E88EA94696}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -625,7 +625,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2000,11 +2000,15 @@
       <c r="E31" s="19">
         <v>43874</v>
       </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="F31" s="19">
+        <v>43879</v>
+      </c>
+      <c r="G31" s="19">
+        <v>43879</v>
+      </c>
       <c r="H31" s="20"/>
       <c r="I31" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="27"/>

</xml_diff>

<commit_message>
Extended the project plan deadlines according to a one day delay in the project timeline Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C720E248-2D24-47B4-AD0B-5B6A550F76FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D237E1-265C-437C-975B-B0270B9FBFD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,13 +171,13 @@
     <t>GDD Documentation</t>
   </si>
   <si>
-    <t>GDD Review and adding points to review sheet</t>
+    <t>Update SRS according to the review sheet and adding what have been resolved to the SRS review sheet and where exactly the points have been resolved</t>
   </si>
   <si>
-    <t>GDD Update according to the review sheet</t>
+    <t>GDD Review and adding points to a new review sheet with the same name as the document name</t>
   </si>
   <si>
-    <t>Update SRS according to the review sheet and adding what have been resolved to the SRS review sheet and where exactly the points have been resolved</t>
+    <t>GDD Update according to the GDD review sheet</t>
   </si>
 </sst>
 </file>
@@ -641,8 +641,8 @@
   <dimension ref="A1:AF1002"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2088,7 +2088,7 @@
     <row r="33" spans="1:32" s="28" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>18</v>
@@ -2137,10 +2137,10 @@
         <v>31</v>
       </c>
       <c r="D34" s="19">
-        <v>43884</v>
+        <v>43886</v>
       </c>
       <c r="E34" s="19">
-        <v>43885</v>
+        <v>43887</v>
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
@@ -2174,16 +2174,16 @@
     <row r="35" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="19">
-        <v>43885</v>
+        <v>43887</v>
       </c>
       <c r="E35" s="19">
-        <v>43885</v>
+        <v>43887</v>
       </c>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
@@ -2217,16 +2217,16 @@
     <row r="36" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30"/>
       <c r="B36" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="19">
-        <v>43885</v>
+        <v>43888</v>
       </c>
       <c r="E36" s="19">
-        <v>43886</v>
+        <v>43888</v>
       </c>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>

</xml_diff>

<commit_message>
Update Project plan according to the command of the team leader Signed-off-by: MS2017A <aeronautics2017@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MS\SWE\SWEGit\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D237E1-265C-437C-975B-B0270B9FBFD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B9B049-6418-42DE-8095-781DB8B060A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PO4_DGELV_Project_Plan" sheetId="1" r:id="rId1"/>
@@ -641,24 +641,24 @@
   <dimension ref="A1:AF1002"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.36328125" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1796875" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
-    <col min="10" max="10" width="9.08984375" customWidth="1"/>
-    <col min="11" max="11" width="50.453125" customWidth="1"/>
-    <col min="12" max="12" width="3.36328125" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="11" width="50.44140625" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" customWidth="1"/>
     <col min="13" max="32" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1265,7 +1265,7 @@
       <c r="AD14" s="3"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:32" s="22" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" s="22" customFormat="1" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="17" t="s">
         <v>27</v>
@@ -1680,7 +1680,7 @@
       <c r="AD23" s="27"/>
       <c r="AE23" s="5"/>
     </row>
-    <row r="24" spans="1:31" s="28" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" s="28" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="17" t="s">
         <v>37</v>
@@ -2099,8 +2099,12 @@
       <c r="E33" s="19">
         <v>43884</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
+      <c r="F33" s="19">
+        <v>43883</v>
+      </c>
+      <c r="G33" s="19">
+        <v>43887</v>
+      </c>
       <c r="H33" s="20"/>
       <c r="I33" s="17" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Adding Week 5 to the projectplan Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MS\SWE\SWEGit\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B9B049-6418-42DE-8095-781DB8B060A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F982E8D-F03D-4DF3-802C-0AC689C95298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PO4_DGELV_Project_Plan" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -179,6 +179,27 @@
   <si>
     <t>GDD Update according to the GDD review sheet</t>
   </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>GDD: Adding Software Context</t>
+  </si>
+  <si>
+    <t>GDD: Adding API Components</t>
+  </si>
+  <si>
+    <t>GDD: Initial Creation + Adding Static Archetecture</t>
+  </si>
+  <si>
+    <t>GDD: Review</t>
+  </si>
+  <si>
+    <t>GDD: Contacting Eng. Tarek for his review</t>
+  </si>
+  <si>
+    <t>GDD: Update according to the review sheet</t>
+  </si>
 </sst>
 </file>
 
@@ -312,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -373,6 +394,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -641,24 +664,24 @@
   <dimension ref="A1:AF1002"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="50.44140625" customWidth="1"/>
-    <col min="12" max="12" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="10" max="10" width="9.08984375" customWidth="1"/>
+    <col min="11" max="11" width="50.453125" customWidth="1"/>
+    <col min="12" max="12" width="3.36328125" customWidth="1"/>
     <col min="13" max="32" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -709,11 +732,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -748,11 +771,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="36"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -782,11 +805,11 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="36"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -1265,7 +1288,7 @@
       <c r="AD14" s="3"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" spans="1:32" s="22" customFormat="1" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" s="22" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="17" t="s">
         <v>27</v>
@@ -1680,7 +1703,7 @@
       <c r="AD23" s="27"/>
       <c r="AE23" s="5"/>
     </row>
-    <row r="24" spans="1:31" s="28" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" s="28" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="17" t="s">
         <v>37</v>
@@ -2261,17 +2284,19 @@
       <c r="AD36" s="27"/>
       <c r="AE36" s="5"/>
     </row>
-    <row r="37" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+    <row r="37" spans="1:32" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
+      <c r="B37" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -2292,212 +2317,265 @@
       <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
-      <c r="AE37" s="3"/>
-      <c r="AF37" s="5"/>
-    </row>
-    <row r="38" spans="1:32" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
-    </row>
-    <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AA39" s="3"/>
-      <c r="AB39" s="3"/>
-      <c r="AC39" s="3"/>
-      <c r="AD39" s="3"/>
-      <c r="AE39" s="3"/>
-      <c r="AF39" s="5"/>
-    </row>
-    <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
-      <c r="W40" s="3"/>
-      <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
-      <c r="AB40" s="3"/>
-      <c r="AC40" s="3"/>
-      <c r="AD40" s="3"/>
-      <c r="AE40" s="3"/>
-      <c r="AF40" s="5"/>
-    </row>
-    <row r="41" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
-      <c r="AA41" s="3"/>
-      <c r="AB41" s="3"/>
-      <c r="AC41" s="3"/>
-      <c r="AD41" s="3"/>
-      <c r="AE41" s="3"/>
-      <c r="AF41" s="5"/>
-    </row>
-    <row r="42" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AA42" s="3"/>
-      <c r="AB42" s="3"/>
-      <c r="AC42" s="3"/>
-      <c r="AD42" s="3"/>
-      <c r="AE42" s="3"/>
-      <c r="AF42" s="5"/>
-    </row>
-    <row r="43" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
-      <c r="W43" s="3"/>
-      <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
-      <c r="AA43" s="3"/>
-      <c r="AB43" s="3"/>
-      <c r="AC43" s="3"/>
-      <c r="AD43" s="3"/>
-      <c r="AE43" s="3"/>
-      <c r="AF43" s="5"/>
+      <c r="AE37" s="5"/>
+    </row>
+    <row r="38" spans="1:32" s="28" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="32"/>
+      <c r="B38" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="19">
+        <v>43890</v>
+      </c>
+      <c r="E38" s="19">
+        <v>43890</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="17"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="27"/>
+      <c r="S38" s="27"/>
+      <c r="T38" s="27"/>
+      <c r="U38" s="27"/>
+      <c r="V38" s="27"/>
+      <c r="W38" s="27"/>
+      <c r="X38" s="27"/>
+      <c r="Y38" s="27"/>
+      <c r="Z38" s="27"/>
+      <c r="AA38" s="27"/>
+      <c r="AB38" s="27"/>
+      <c r="AC38" s="27"/>
+      <c r="AD38" s="27"/>
+      <c r="AE38" s="5"/>
+    </row>
+    <row r="39" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="32"/>
+      <c r="B39" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="19">
+        <v>43891</v>
+      </c>
+      <c r="E39" s="19">
+        <v>43891</v>
+      </c>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="17"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="27"/>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="27"/>
+      <c r="W39" s="27"/>
+      <c r="X39" s="27"/>
+      <c r="Y39" s="27"/>
+      <c r="Z39" s="27"/>
+      <c r="AA39" s="27"/>
+      <c r="AB39" s="27"/>
+      <c r="AC39" s="27"/>
+      <c r="AD39" s="27"/>
+      <c r="AE39" s="5"/>
+    </row>
+    <row r="40" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="32"/>
+      <c r="B40" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="19">
+        <v>43892</v>
+      </c>
+      <c r="E40" s="19">
+        <v>43893</v>
+      </c>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="17"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27"/>
+      <c r="U40" s="27"/>
+      <c r="V40" s="27"/>
+      <c r="W40" s="27"/>
+      <c r="X40" s="27"/>
+      <c r="Y40" s="27"/>
+      <c r="Z40" s="27"/>
+      <c r="AA40" s="27"/>
+      <c r="AB40" s="27"/>
+      <c r="AC40" s="27"/>
+      <c r="AD40" s="27"/>
+      <c r="AE40" s="5"/>
+    </row>
+    <row r="41" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32"/>
+      <c r="B41" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="19">
+        <v>43893</v>
+      </c>
+      <c r="E41" s="19">
+        <v>43894</v>
+      </c>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J41" s="17"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27"/>
+      <c r="U41" s="27"/>
+      <c r="V41" s="27"/>
+      <c r="W41" s="27"/>
+      <c r="X41" s="27"/>
+      <c r="Y41" s="27"/>
+      <c r="Z41" s="27"/>
+      <c r="AA41" s="27"/>
+      <c r="AB41" s="27"/>
+      <c r="AC41" s="27"/>
+      <c r="AD41" s="27"/>
+      <c r="AE41" s="5"/>
+    </row>
+    <row r="42" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="32"/>
+      <c r="B42" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="19">
+        <v>43894</v>
+      </c>
+      <c r="E42" s="19">
+        <v>43894</v>
+      </c>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J42" s="17"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="27"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="27"/>
+      <c r="Q42" s="27"/>
+      <c r="R42" s="27"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="27"/>
+      <c r="U42" s="27"/>
+      <c r="V42" s="27"/>
+      <c r="W42" s="27"/>
+      <c r="X42" s="27"/>
+      <c r="Y42" s="27"/>
+      <c r="Z42" s="27"/>
+      <c r="AA42" s="27"/>
+      <c r="AB42" s="27"/>
+      <c r="AC42" s="27"/>
+      <c r="AD42" s="27"/>
+      <c r="AE42" s="5"/>
+    </row>
+    <row r="43" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="32"/>
+      <c r="B43" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="19">
+        <v>43895</v>
+      </c>
+      <c r="E43" s="19">
+        <v>43895</v>
+      </c>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J43" s="17"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="27"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="27"/>
+      <c r="Q43" s="27"/>
+      <c r="R43" s="27"/>
+      <c r="S43" s="27"/>
+      <c r="T43" s="27"/>
+      <c r="U43" s="27"/>
+      <c r="V43" s="27"/>
+      <c r="W43" s="27"/>
+      <c r="X43" s="27"/>
+      <c r="Y43" s="27"/>
+      <c r="Z43" s="27"/>
+      <c r="AA43" s="27"/>
+      <c r="AB43" s="27"/>
+      <c r="AC43" s="27"/>
+      <c r="AD43" s="27"/>
+      <c r="AE43" s="5"/>
     </row>
     <row r="44" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -35110,7 +35188,7 @@
     <mergeCell ref="G2:K4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I24 I26:I31 I33:I36" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I24 I26:I31 I33:I36 I38:I43" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Assigned,Started,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added CDD documentation to the plan Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
+++ b/Digital_Elevator_PO4_DGELV/SW deliveries log/Project Plan/PO4_DGELV_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\SW deliveries log\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F982E8D-F03D-4DF3-802C-0AC689C95298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D10151E-842F-4F88-8E17-01D3CED6B4A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -200,6 +200,12 @@
   <si>
     <t>GDD: Update according to the review sheet</t>
   </si>
+  <si>
+    <t>CDD Initial Creation</t>
+  </si>
+  <si>
+    <t>Mostafa Sayed</t>
+  </si>
 </sst>
 </file>
 
@@ -333,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -398,6 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -661,11 +668,11 @@
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF1002"/>
+  <dimension ref="A1:AF1003"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -732,11 +739,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="37"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -771,11 +778,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -805,11 +812,11 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="39"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -2417,7 +2424,7 @@
         <v>43892</v>
       </c>
       <c r="E40" s="19">
-        <v>43893</v>
+        <v>43892</v>
       </c>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
@@ -2460,7 +2467,7 @@
         <v>43893</v>
       </c>
       <c r="E41" s="19">
-        <v>43894</v>
+        <v>43893</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
@@ -2491,19 +2498,19 @@
       <c r="AD41" s="27"/>
       <c r="AE41" s="5"/>
     </row>
-    <row r="42" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+    <row r="42" spans="1:32" s="28" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
       <c r="B42" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="D42" s="19">
-        <v>43894</v>
+        <v>43893</v>
       </c>
       <c r="E42" s="19">
-        <v>43894</v>
+        <v>43895</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -2537,16 +2544,16 @@
     <row r="43" spans="1:32" s="28" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="32"/>
       <c r="B43" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D43" s="19">
-        <v>43895</v>
+        <v>43894</v>
       </c>
       <c r="E43" s="19">
-        <v>43895</v>
+        <v>43894</v>
       </c>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
@@ -2577,73 +2584,48 @@
       <c r="AD43" s="27"/>
       <c r="AE43" s="5"/>
     </row>
-    <row r="44" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
-      <c r="AA44" s="3"/>
-      <c r="AB44" s="3"/>
-      <c r="AC44" s="3"/>
-      <c r="AD44" s="3"/>
-      <c r="AE44" s="3"/>
-      <c r="AF44" s="5"/>
-    </row>
-    <row r="45" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="3"/>
-      <c r="Y45" s="3"/>
-      <c r="Z45" s="3"/>
-      <c r="AA45" s="3"/>
-      <c r="AB45" s="3"/>
-      <c r="AC45" s="3"/>
-      <c r="AD45" s="3"/>
-      <c r="AE45" s="3"/>
-      <c r="AF45" s="5"/>
+    <row r="44" spans="1:32" s="28" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32"/>
+      <c r="B44" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="19">
+        <v>43895</v>
+      </c>
+      <c r="E44" s="19">
+        <v>43895</v>
+      </c>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="17"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+      <c r="N44" s="27"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="27"/>
+      <c r="Q44" s="27"/>
+      <c r="R44" s="27"/>
+      <c r="S44" s="27"/>
+      <c r="T44" s="27"/>
+      <c r="U44" s="27"/>
+      <c r="V44" s="27"/>
+      <c r="W44" s="27"/>
+      <c r="X44" s="27"/>
+      <c r="Y44" s="27"/>
+      <c r="Z44" s="27"/>
+      <c r="AA44" s="27"/>
+      <c r="AB44" s="27"/>
+      <c r="AC44" s="27"/>
+      <c r="AD44" s="27"/>
+      <c r="AE44" s="5"/>
     </row>
     <row r="46" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
@@ -8665,37 +8647,37 @@
     </row>
     <row r="223" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
-      <c r="D223" s="1"/>
-      <c r="E223" s="1"/>
-      <c r="F223" s="1"/>
-      <c r="G223" s="1"/>
-      <c r="H223" s="1"/>
-      <c r="I223" s="1"/>
-      <c r="J223" s="1"/>
-      <c r="K223" s="1"/>
-      <c r="L223" s="1"/>
-      <c r="M223" s="1"/>
-      <c r="N223" s="1"/>
-      <c r="O223" s="1"/>
-      <c r="P223" s="1"/>
-      <c r="Q223" s="1"/>
-      <c r="R223" s="1"/>
-      <c r="S223" s="1"/>
-      <c r="T223" s="1"/>
-      <c r="U223" s="1"/>
-      <c r="V223" s="1"/>
-      <c r="W223" s="1"/>
-      <c r="X223" s="1"/>
-      <c r="Y223" s="1"/>
-      <c r="Z223" s="1"/>
-      <c r="AA223" s="1"/>
-      <c r="AB223" s="1"/>
-      <c r="AC223" s="1"/>
-      <c r="AD223" s="1"/>
-      <c r="AE223" s="1"/>
-      <c r="AF223" s="1"/>
+      <c r="B223" s="3"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="3"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
+      <c r="H223" s="3"/>
+      <c r="I223" s="3"/>
+      <c r="J223" s="3"/>
+      <c r="K223" s="3"/>
+      <c r="L223" s="3"/>
+      <c r="M223" s="3"/>
+      <c r="N223" s="3"/>
+      <c r="O223" s="3"/>
+      <c r="P223" s="3"/>
+      <c r="Q223" s="3"/>
+      <c r="R223" s="3"/>
+      <c r="S223" s="3"/>
+      <c r="T223" s="3"/>
+      <c r="U223" s="3"/>
+      <c r="V223" s="3"/>
+      <c r="W223" s="3"/>
+      <c r="X223" s="3"/>
+      <c r="Y223" s="3"/>
+      <c r="Z223" s="3"/>
+      <c r="AA223" s="3"/>
+      <c r="AB223" s="3"/>
+      <c r="AC223" s="3"/>
+      <c r="AD223" s="3"/>
+      <c r="AE223" s="3"/>
+      <c r="AF223" s="5"/>
     </row>
     <row r="224" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
@@ -35183,12 +35165,46 @@
       <c r="AE1002" s="1"/>
       <c r="AF1002" s="1"/>
     </row>
+    <row r="1003" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+      <c r="AA1003" s="1"/>
+      <c r="AB1003" s="1"/>
+      <c r="AC1003" s="1"/>
+      <c r="AD1003" s="1"/>
+      <c r="AE1003" s="1"/>
+      <c r="AF1003" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G2:K4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I24 I26:I31 I33:I36 I38:I43" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I8:I15 I17:I24 I26:I31 I33:I36 I38:I44" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Assigned,Started,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>